<commit_message>
Control categories from presenterview
</commit_message>
<xml_diff>
--- a/public/quiz/asd.xlsx
+++ b/public/quiz/asd.xlsx
@@ -14,15 +14,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="98">
   <si>
     <t>name</t>
   </si>
   <si>
+    <t>Image</t>
+  </si>
+  <si>
     <t>Adams 25</t>
   </si>
   <si>
-    <t>Table 1</t>
+    <t>able 1</t>
   </si>
   <si>
     <t>Categories</t>
@@ -1039,7 +1042,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -2278,7 +2281,9 @@
       <c r="E1" s="3"/>
     </row>
     <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" s="4"/>
+      <c r="A2" t="s" s="4">
+        <v>2</v>
+      </c>
       <c r="B2" s="5"/>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -2368,7 +2373,7 @@
   <sheetData>
     <row r="1" ht="14.6" customHeight="1">
       <c r="A1" t="s" s="11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -2474,325 +2479,325 @@
   <sheetData>
     <row r="1" ht="32.25" customHeight="1">
       <c r="A1" t="s" s="20">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s" s="21">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s" s="21">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s" s="21">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E1" t="s" s="21">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F1" t="s" s="21">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G1" t="s" s="21">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H1" t="s" s="21">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I1" t="s" s="21">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J1" t="s" s="21">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K1" t="s" s="21">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L1" t="s" s="21">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="M1" t="s" s="21">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N1" t="s" s="21">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O1" t="s" s="21">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" ht="100.2" customHeight="1">
       <c r="A2" t="s" s="22">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s" s="23">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s" s="24">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s" s="24">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E2" t="s" s="24">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F2" t="s" s="24">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s" s="24">
+        <v>25</v>
+      </c>
+      <c r="H2" t="s" s="24">
         <v>23</v>
       </c>
-      <c r="G2" t="s" s="24">
-        <v>24</v>
-      </c>
-      <c r="H2" t="s" s="24">
-        <v>22</v>
-      </c>
       <c r="I2" t="s" s="24">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J2" t="s" s="24">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K2" t="s" s="24">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L2" t="s" s="24">
+        <v>28</v>
+      </c>
+      <c r="M2" t="s" s="24">
         <v>27</v>
       </c>
-      <c r="M2" t="s" s="24">
-        <v>26</v>
-      </c>
       <c r="N2" t="s" s="24">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O2" s="25"/>
     </row>
     <row r="3" ht="100.45" customHeight="1">
       <c r="A3" t="s" s="26">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s" s="27">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s" s="28">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s" s="28">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E3" t="s" s="28">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F3" t="s" s="28">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G3" t="s" s="28">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H3" t="s" s="28">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I3" t="s" s="28">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J3" t="s" s="28">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K3" t="s" s="28">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L3" t="s" s="28">
+        <v>37</v>
+      </c>
+      <c r="M3" t="s" s="28">
         <v>36</v>
       </c>
-      <c r="M3" t="s" s="28">
-        <v>35</v>
-      </c>
       <c r="N3" t="s" s="28">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O3" s="29"/>
     </row>
     <row r="4" ht="100.45" customHeight="1">
       <c r="A4" t="s" s="26">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s" s="27">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s" s="28">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D4" t="s" s="28">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E4" t="s" s="30">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F4" t="s" s="31">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G4" t="s" s="28">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H4" t="s" s="28">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I4" t="s" s="28">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J4" t="s" s="28">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K4" t="s" s="28">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L4" t="s" s="28">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M4" t="s" s="28">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="N4" t="s" s="28">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O4" s="29"/>
     </row>
     <row r="5" ht="100.45" customHeight="1">
       <c r="A5" t="s" s="26">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s" s="27">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C5" t="s" s="28">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s" s="28">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E5" t="s" s="28">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F5" t="s" s="28">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G5" t="s" s="28">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H5" t="s" s="28">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I5" s="32">
         <v>2014</v>
       </c>
       <c r="J5" t="s" s="28">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K5" t="s" s="28">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L5" t="s" s="28">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="M5" t="s" s="28">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="N5" t="s" s="28">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O5" t="s" s="28">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" ht="100.45" customHeight="1">
       <c r="A6" t="s" s="26">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B6" t="s" s="27">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C6" t="s" s="28">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D6" t="s" s="28">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E6" t="s" s="28">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F6" t="s" s="28">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G6" t="s" s="28">
+        <v>63</v>
+      </c>
+      <c r="H6" t="s" s="28">
+        <v>23</v>
+      </c>
+      <c r="I6" t="s" s="28">
         <v>62</v>
       </c>
-      <c r="H6" t="s" s="28">
-        <v>22</v>
-      </c>
-      <c r="I6" t="s" s="28">
-        <v>61</v>
-      </c>
       <c r="J6" t="s" s="28">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K6" t="s" s="28">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L6" t="s" s="28">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="M6" t="s" s="28">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="N6" t="s" s="28">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O6" t="s" s="28">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" ht="100.45" customHeight="1">
       <c r="A7" t="s" s="26">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B7" t="s" s="33">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C7" t="s" s="28">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D7" t="s" s="28">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E7" t="s" s="28">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F7" t="s" s="28">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G7" t="s" s="28">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H7" t="s" s="28">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I7" t="s" s="28">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J7" t="s" s="28">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="K7" t="s" s="28">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L7" t="s" s="28">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="M7" t="s" s="28">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="N7" t="s" s="28">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O7" t="s" s="28">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" ht="65.35" customHeight="1">
@@ -3043,91 +3048,91 @@
   <sheetData>
     <row r="1" ht="100" customHeight="1">
       <c r="A1" t="s" s="20">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B1" t="s" s="21">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s" s="21">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s" s="21">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E1" t="s" s="21">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F1" t="s" s="21">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G1" t="s" s="21">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H1" t="s" s="21">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I1" t="s" s="21">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J1" t="s" s="21">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K1" t="s" s="21">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L1" t="s" s="21">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="M1" t="s" s="21">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N1" t="s" s="21">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O1" t="s" s="21">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" ht="100" customHeight="1">
       <c r="A2" t="s" s="22">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s" s="39">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C2" t="s" s="40">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D2" t="s" s="40">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E2" s="41"/>
       <c r="F2" s="41"/>
       <c r="G2" t="s" s="40">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H2" s="41"/>
       <c r="I2" s="41"/>
       <c r="J2" t="s" s="40">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K2" s="41"/>
       <c r="L2" s="41"/>
       <c r="M2" t="s" s="40">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="N2" s="42"/>
       <c r="O2" s="42"/>
     </row>
     <row r="3" ht="100" customHeight="1">
       <c r="A3" t="s" s="26">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B3" t="s" s="36">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C3" t="s" s="43">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D3" s="44"/>
       <c r="E3" s="44"/>
@@ -3144,13 +3149,13 @@
     </row>
     <row r="4" ht="100" customHeight="1">
       <c r="A4" t="s" s="26">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B4" t="s" s="36">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C4" t="s" s="43">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D4" s="45"/>
       <c r="E4" s="45"/>
@@ -3167,31 +3172,31 @@
     </row>
     <row r="5" ht="100" customHeight="1">
       <c r="A5" t="s" s="26">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B5" t="s" s="36">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C5" t="s" s="43">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D5" t="s" s="43">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E5" s="45"/>
       <c r="F5" s="45"/>
       <c r="G5" t="s" s="43">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H5" s="45"/>
       <c r="I5" s="45"/>
       <c r="J5" t="s" s="43">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K5" s="45"/>
       <c r="L5" s="45"/>
       <c r="M5" t="s" s="43">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="N5" s="45"/>
       <c r="O5" s="45"/>

</xml_diff>

<commit_message>
Sync teams from excel file
</commit_message>
<xml_diff>
--- a/public/quiz/asd.xlsx
+++ b/public/quiz/asd.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="107">
   <si>
     <t>name</t>
   </si>
@@ -25,7 +25,34 @@
     <t>Adams 25</t>
   </si>
   <si>
-    <t>able 1</t>
+    <t>Lagnamn</t>
+  </si>
+  <si>
+    <t>Lads</t>
+  </si>
+  <si>
+    <t>Adam</t>
+  </si>
+  <si>
+    <t>Gson</t>
+  </si>
+  <si>
+    <t>Lag 2</t>
+  </si>
+  <si>
+    <t>W6</t>
+  </si>
+  <si>
+    <t>Fiddman</t>
+  </si>
+  <si>
+    <t>Lag 3</t>
+  </si>
+  <si>
+    <t>Chris</t>
+  </si>
+  <si>
+    <t>Beckson</t>
   </si>
   <si>
     <t>Categories</t>
@@ -1029,7 +1056,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1063,28 +1090,40 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -2359,10 +2398,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:E11"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
+      <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozen"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2371,89 +2410,97 @@
     <col min="6" max="16384" width="16.3516" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.6" customHeight="1">
+    <row r="1" ht="14.25" customHeight="1">
       <c r="A1" t="s" s="11">
         <v>3</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-    </row>
-    <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="13"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
+      <c r="A2" t="s" s="13">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s" s="14">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s" s="15">
+        <v>6</v>
+      </c>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+    </row>
+    <row r="3" ht="14.05" customHeight="1">
+      <c r="A3" t="s" s="17">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s" s="18">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s" s="19">
+        <v>9</v>
+      </c>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
     </row>
     <row r="4" ht="14.05" customHeight="1">
-      <c r="A4" s="16"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
+      <c r="A4" t="s" s="17">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s" s="18">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s" s="19">
+        <v>12</v>
+      </c>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
     </row>
     <row r="5" ht="14.05" customHeight="1">
-      <c r="A5" s="16"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
+      <c r="A5" s="21"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
     </row>
     <row r="6" ht="14.05" customHeight="1">
-      <c r="A6" s="16"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
+      <c r="A6" s="21"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
     </row>
     <row r="7" ht="14.05" customHeight="1">
-      <c r="A7" s="16"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
+      <c r="A7" s="21"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
     </row>
     <row r="8" ht="14.05" customHeight="1">
-      <c r="A8" s="16"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
     </row>
     <row r="9" ht="14.05" customHeight="1">
-      <c r="A9" s="16"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
+      <c r="A9" s="21"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
     </row>
     <row r="10" ht="14.05" customHeight="1">
-      <c r="A10" s="16"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-    </row>
-    <row r="11" ht="14.05" customHeight="1">
-      <c r="A11" s="16"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
+      <c r="A10" s="21"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
-  </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
@@ -2470,334 +2517,334 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="29.5" style="19" customWidth="1"/>
-    <col min="2" max="8" width="16.3516" style="19" customWidth="1"/>
-    <col min="9" max="9" width="56.1719" style="19" customWidth="1"/>
-    <col min="10" max="15" width="16.3516" style="19" customWidth="1"/>
-    <col min="16" max="16384" width="16.3516" style="19" customWidth="1"/>
+    <col min="1" max="1" width="29.5" style="23" customWidth="1"/>
+    <col min="2" max="8" width="16.3516" style="23" customWidth="1"/>
+    <col min="9" max="9" width="56.1719" style="23" customWidth="1"/>
+    <col min="10" max="15" width="16.3516" style="23" customWidth="1"/>
+    <col min="16" max="16384" width="16.3516" style="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="32.25" customHeight="1">
-      <c r="A1" t="s" s="20">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s" s="21">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s" s="21">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s" s="21">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s" s="21">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s" s="21">
-        <v>9</v>
-      </c>
-      <c r="G1" t="s" s="21">
-        <v>10</v>
-      </c>
-      <c r="H1" t="s" s="21">
-        <v>11</v>
-      </c>
-      <c r="I1" t="s" s="21">
-        <v>12</v>
-      </c>
-      <c r="J1" t="s" s="21">
+      <c r="A1" t="s" s="24">
         <v>13</v>
       </c>
-      <c r="K1" t="s" s="21">
+      <c r="B1" t="s" s="25">
         <v>14</v>
       </c>
-      <c r="L1" t="s" s="21">
+      <c r="C1" t="s" s="25">
         <v>15</v>
       </c>
-      <c r="M1" t="s" s="21">
+      <c r="D1" t="s" s="25">
         <v>16</v>
       </c>
-      <c r="N1" t="s" s="21">
+      <c r="E1" t="s" s="25">
         <v>17</v>
       </c>
-      <c r="O1" t="s" s="21">
+      <c r="F1" t="s" s="25">
         <v>18</v>
       </c>
+      <c r="G1" t="s" s="25">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s" s="25">
+        <v>20</v>
+      </c>
+      <c r="I1" t="s" s="25">
+        <v>21</v>
+      </c>
+      <c r="J1" t="s" s="25">
+        <v>22</v>
+      </c>
+      <c r="K1" t="s" s="25">
+        <v>23</v>
+      </c>
+      <c r="L1" t="s" s="25">
+        <v>24</v>
+      </c>
+      <c r="M1" t="s" s="25">
+        <v>25</v>
+      </c>
+      <c r="N1" t="s" s="25">
+        <v>26</v>
+      </c>
+      <c r="O1" t="s" s="25">
+        <v>27</v>
+      </c>
     </row>
     <row r="2" ht="100.2" customHeight="1">
-      <c r="A2" t="s" s="22">
-        <v>19</v>
-      </c>
-      <c r="B2" t="s" s="23">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s" s="24">
-        <v>21</v>
-      </c>
-      <c r="D2" t="s" s="24">
-        <v>22</v>
-      </c>
-      <c r="E2" t="s" s="24">
-        <v>23</v>
-      </c>
-      <c r="F2" t="s" s="24">
-        <v>24</v>
-      </c>
-      <c r="G2" t="s" s="24">
-        <v>25</v>
-      </c>
-      <c r="H2" t="s" s="24">
-        <v>23</v>
-      </c>
-      <c r="I2" t="s" s="24">
-        <v>26</v>
-      </c>
-      <c r="J2" t="s" s="24">
-        <v>27</v>
-      </c>
-      <c r="K2" t="s" s="24">
-        <v>23</v>
-      </c>
-      <c r="L2" t="s" s="24">
+      <c r="A2" t="s" s="26">
         <v>28</v>
       </c>
-      <c r="M2" t="s" s="24">
-        <v>27</v>
-      </c>
-      <c r="N2" t="s" s="24">
-        <v>23</v>
-      </c>
-      <c r="O2" s="25"/>
+      <c r="B2" t="s" s="27">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s" s="28">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s" s="28">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s" s="28">
+        <v>32</v>
+      </c>
+      <c r="F2" t="s" s="28">
+        <v>33</v>
+      </c>
+      <c r="G2" t="s" s="28">
+        <v>34</v>
+      </c>
+      <c r="H2" t="s" s="28">
+        <v>32</v>
+      </c>
+      <c r="I2" t="s" s="28">
+        <v>35</v>
+      </c>
+      <c r="J2" t="s" s="28">
+        <v>36</v>
+      </c>
+      <c r="K2" t="s" s="28">
+        <v>32</v>
+      </c>
+      <c r="L2" t="s" s="28">
+        <v>37</v>
+      </c>
+      <c r="M2" t="s" s="28">
+        <v>36</v>
+      </c>
+      <c r="N2" t="s" s="28">
+        <v>32</v>
+      </c>
+      <c r="O2" s="29"/>
     </row>
     <row r="3" ht="100.45" customHeight="1">
-      <c r="A3" t="s" s="26">
-        <v>29</v>
-      </c>
-      <c r="B3" t="s" s="27">
-        <v>30</v>
-      </c>
-      <c r="C3" t="s" s="28">
-        <v>31</v>
-      </c>
-      <c r="D3" t="s" s="28">
+      <c r="A3" t="s" s="30">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s" s="31">
+        <v>39</v>
+      </c>
+      <c r="C3" t="s" s="32">
+        <v>40</v>
+      </c>
+      <c r="D3" t="s" s="32">
+        <v>41</v>
+      </c>
+      <c r="E3" t="s" s="32">
         <v>32</v>
       </c>
-      <c r="E3" t="s" s="28">
-        <v>23</v>
-      </c>
-      <c r="F3" t="s" s="28">
-        <v>33</v>
-      </c>
-      <c r="G3" t="s" s="28">
-        <v>34</v>
-      </c>
-      <c r="H3" t="s" s="28">
-        <v>23</v>
-      </c>
-      <c r="I3" t="s" s="28">
-        <v>35</v>
-      </c>
-      <c r="J3" t="s" s="28">
-        <v>36</v>
-      </c>
-      <c r="K3" t="s" s="28">
-        <v>23</v>
-      </c>
-      <c r="L3" t="s" s="28">
-        <v>37</v>
-      </c>
-      <c r="M3" t="s" s="28">
-        <v>36</v>
-      </c>
-      <c r="N3" t="s" s="28">
-        <v>23</v>
-      </c>
-      <c r="O3" s="29"/>
+      <c r="F3" t="s" s="32">
+        <v>42</v>
+      </c>
+      <c r="G3" t="s" s="32">
+        <v>43</v>
+      </c>
+      <c r="H3" t="s" s="32">
+        <v>32</v>
+      </c>
+      <c r="I3" t="s" s="32">
+        <v>44</v>
+      </c>
+      <c r="J3" t="s" s="32">
+        <v>45</v>
+      </c>
+      <c r="K3" t="s" s="32">
+        <v>32</v>
+      </c>
+      <c r="L3" t="s" s="32">
+        <v>46</v>
+      </c>
+      <c r="M3" t="s" s="32">
+        <v>45</v>
+      </c>
+      <c r="N3" t="s" s="32">
+        <v>32</v>
+      </c>
+      <c r="O3" s="33"/>
     </row>
     <row r="4" ht="100.45" customHeight="1">
-      <c r="A4" t="s" s="26">
-        <v>38</v>
-      </c>
-      <c r="B4" t="s" s="27">
-        <v>39</v>
-      </c>
-      <c r="C4" t="s" s="28">
-        <v>40</v>
-      </c>
-      <c r="D4" t="s" s="28">
-        <v>41</v>
-      </c>
-      <c r="E4" t="s" s="30">
-        <v>23</v>
-      </c>
-      <c r="F4" t="s" s="31">
-        <v>42</v>
-      </c>
-      <c r="G4" t="s" s="28">
-        <v>43</v>
-      </c>
-      <c r="H4" t="s" s="28">
-        <v>23</v>
-      </c>
-      <c r="I4" t="s" s="28">
-        <v>44</v>
-      </c>
-      <c r="J4" t="s" s="28">
-        <v>45</v>
-      </c>
-      <c r="K4" t="s" s="28">
-        <v>23</v>
-      </c>
-      <c r="L4" t="s" s="28">
-        <v>46</v>
-      </c>
-      <c r="M4" t="s" s="28">
+      <c r="A4" t="s" s="30">
         <v>47</v>
       </c>
-      <c r="N4" t="s" s="28">
-        <v>23</v>
-      </c>
-      <c r="O4" s="29"/>
+      <c r="B4" t="s" s="31">
+        <v>48</v>
+      </c>
+      <c r="C4" t="s" s="32">
+        <v>49</v>
+      </c>
+      <c r="D4" t="s" s="32">
+        <v>50</v>
+      </c>
+      <c r="E4" t="s" s="34">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s" s="35">
+        <v>51</v>
+      </c>
+      <c r="G4" t="s" s="32">
+        <v>52</v>
+      </c>
+      <c r="H4" t="s" s="32">
+        <v>32</v>
+      </c>
+      <c r="I4" t="s" s="32">
+        <v>53</v>
+      </c>
+      <c r="J4" t="s" s="32">
+        <v>54</v>
+      </c>
+      <c r="K4" t="s" s="32">
+        <v>32</v>
+      </c>
+      <c r="L4" t="s" s="32">
+        <v>55</v>
+      </c>
+      <c r="M4" t="s" s="32">
+        <v>56</v>
+      </c>
+      <c r="N4" t="s" s="32">
+        <v>32</v>
+      </c>
+      <c r="O4" s="33"/>
     </row>
     <row r="5" ht="100.45" customHeight="1">
-      <c r="A5" t="s" s="26">
-        <v>48</v>
-      </c>
-      <c r="B5" t="s" s="27">
-        <v>49</v>
-      </c>
-      <c r="C5" t="s" s="28">
-        <v>50</v>
-      </c>
-      <c r="D5" t="s" s="28">
-        <v>51</v>
-      </c>
-      <c r="E5" t="s" s="28">
-        <v>23</v>
-      </c>
-      <c r="F5" t="s" s="28">
-        <v>52</v>
-      </c>
-      <c r="G5" t="s" s="28">
-        <v>53</v>
-      </c>
-      <c r="H5" t="s" s="28">
-        <v>23</v>
-      </c>
-      <c r="I5" s="32">
+      <c r="A5" t="s" s="30">
+        <v>57</v>
+      </c>
+      <c r="B5" t="s" s="31">
+        <v>58</v>
+      </c>
+      <c r="C5" t="s" s="32">
+        <v>59</v>
+      </c>
+      <c r="D5" t="s" s="32">
+        <v>60</v>
+      </c>
+      <c r="E5" t="s" s="32">
+        <v>32</v>
+      </c>
+      <c r="F5" t="s" s="32">
+        <v>61</v>
+      </c>
+      <c r="G5" t="s" s="32">
+        <v>62</v>
+      </c>
+      <c r="H5" t="s" s="32">
+        <v>32</v>
+      </c>
+      <c r="I5" s="36">
         <v>2014</v>
       </c>
-      <c r="J5" t="s" s="28">
-        <v>54</v>
-      </c>
-      <c r="K5" t="s" s="28">
-        <v>23</v>
-      </c>
-      <c r="L5" t="s" s="28">
-        <v>55</v>
-      </c>
-      <c r="M5" t="s" s="28">
-        <v>56</v>
-      </c>
-      <c r="N5" t="s" s="28">
-        <v>23</v>
-      </c>
-      <c r="O5" t="s" s="28">
-        <v>57</v>
+      <c r="J5" t="s" s="32">
+        <v>63</v>
+      </c>
+      <c r="K5" t="s" s="32">
+        <v>32</v>
+      </c>
+      <c r="L5" t="s" s="32">
+        <v>64</v>
+      </c>
+      <c r="M5" t="s" s="32">
+        <v>65</v>
+      </c>
+      <c r="N5" t="s" s="32">
+        <v>32</v>
+      </c>
+      <c r="O5" t="s" s="32">
+        <v>66</v>
       </c>
     </row>
     <row r="6" ht="100.45" customHeight="1">
-      <c r="A6" t="s" s="26">
-        <v>58</v>
-      </c>
-      <c r="B6" t="s" s="27">
-        <v>59</v>
-      </c>
-      <c r="C6" t="s" s="28">
-        <v>60</v>
-      </c>
-      <c r="D6" t="s" s="28">
-        <v>61</v>
-      </c>
-      <c r="E6" t="s" s="28">
-        <v>23</v>
-      </c>
-      <c r="F6" t="s" s="28">
-        <v>62</v>
-      </c>
-      <c r="G6" t="s" s="28">
-        <v>63</v>
-      </c>
-      <c r="H6" t="s" s="28">
-        <v>23</v>
-      </c>
-      <c r="I6" t="s" s="28">
-        <v>62</v>
-      </c>
-      <c r="J6" t="s" s="28">
-        <v>64</v>
-      </c>
-      <c r="K6" t="s" s="28">
-        <v>23</v>
-      </c>
-      <c r="L6" t="s" s="28">
-        <v>62</v>
-      </c>
-      <c r="M6" t="s" s="28">
-        <v>65</v>
-      </c>
-      <c r="N6" t="s" s="28">
-        <v>23</v>
-      </c>
-      <c r="O6" t="s" s="28">
-        <v>62</v>
+      <c r="A6" t="s" s="30">
+        <v>67</v>
+      </c>
+      <c r="B6" t="s" s="31">
+        <v>68</v>
+      </c>
+      <c r="C6" t="s" s="32">
+        <v>69</v>
+      </c>
+      <c r="D6" t="s" s="32">
+        <v>70</v>
+      </c>
+      <c r="E6" t="s" s="32">
+        <v>32</v>
+      </c>
+      <c r="F6" t="s" s="32">
+        <v>71</v>
+      </c>
+      <c r="G6" t="s" s="32">
+        <v>72</v>
+      </c>
+      <c r="H6" t="s" s="32">
+        <v>32</v>
+      </c>
+      <c r="I6" t="s" s="32">
+        <v>71</v>
+      </c>
+      <c r="J6" t="s" s="32">
+        <v>73</v>
+      </c>
+      <c r="K6" t="s" s="32">
+        <v>32</v>
+      </c>
+      <c r="L6" t="s" s="32">
+        <v>71</v>
+      </c>
+      <c r="M6" t="s" s="32">
+        <v>74</v>
+      </c>
+      <c r="N6" t="s" s="32">
+        <v>32</v>
+      </c>
+      <c r="O6" t="s" s="32">
+        <v>71</v>
       </c>
     </row>
     <row r="7" ht="100.45" customHeight="1">
-      <c r="A7" t="s" s="26">
-        <v>66</v>
-      </c>
-      <c r="B7" t="s" s="33">
-        <v>67</v>
-      </c>
-      <c r="C7" t="s" s="28">
-        <v>68</v>
-      </c>
-      <c r="D7" t="s" s="28">
-        <v>69</v>
-      </c>
-      <c r="E7" t="s" s="28">
-        <v>23</v>
-      </c>
-      <c r="F7" t="s" s="28">
-        <v>70</v>
-      </c>
-      <c r="G7" t="s" s="28">
-        <v>71</v>
-      </c>
-      <c r="H7" t="s" s="28">
-        <v>23</v>
-      </c>
-      <c r="I7" t="s" s="28">
-        <v>72</v>
-      </c>
-      <c r="J7" t="s" s="28">
-        <v>73</v>
-      </c>
-      <c r="K7" t="s" s="28">
-        <v>23</v>
-      </c>
-      <c r="L7" t="s" s="28">
-        <v>74</v>
-      </c>
-      <c r="M7" t="s" s="28">
+      <c r="A7" t="s" s="30">
         <v>75</v>
       </c>
-      <c r="N7" t="s" s="28">
-        <v>23</v>
-      </c>
-      <c r="O7" t="s" s="28">
+      <c r="B7" t="s" s="37">
         <v>76</v>
+      </c>
+      <c r="C7" t="s" s="32">
+        <v>77</v>
+      </c>
+      <c r="D7" t="s" s="32">
+        <v>78</v>
+      </c>
+      <c r="E7" t="s" s="32">
+        <v>32</v>
+      </c>
+      <c r="F7" t="s" s="32">
+        <v>79</v>
+      </c>
+      <c r="G7" t="s" s="32">
+        <v>80</v>
+      </c>
+      <c r="H7" t="s" s="32">
+        <v>32</v>
+      </c>
+      <c r="I7" t="s" s="32">
+        <v>81</v>
+      </c>
+      <c r="J7" t="s" s="32">
+        <v>82</v>
+      </c>
+      <c r="K7" t="s" s="32">
+        <v>32</v>
+      </c>
+      <c r="L7" t="s" s="32">
+        <v>83</v>
+      </c>
+      <c r="M7" t="s" s="32">
+        <v>84</v>
+      </c>
+      <c r="N7" t="s" s="32">
+        <v>32</v>
+      </c>
+      <c r="O7" t="s" s="32">
+        <v>85</v>
       </c>
     </row>
     <row r="8" ht="65.35" customHeight="1">
@@ -2809,7 +2856,7 @@
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
-      <c r="I8" s="34"/>
+      <c r="I8" s="38"/>
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
@@ -2818,7 +2865,7 @@
       <c r="O8" s="9"/>
     </row>
     <row r="9" ht="31.75" customHeight="1">
-      <c r="A9" s="35"/>
+      <c r="A9" s="39"/>
       <c r="B9" s="8"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
@@ -2835,43 +2882,43 @@
       <c r="O9" s="9"/>
     </row>
     <row r="10" ht="100" customHeight="1">
-      <c r="A10" s="26"/>
-      <c r="B10" s="36"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="28"/>
-      <c r="K10" s="29"/>
-      <c r="L10" s="29"/>
-      <c r="M10" s="28"/>
+      <c r="A10" s="30"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="33"/>
+      <c r="L10" s="33"/>
+      <c r="M10" s="32"/>
       <c r="N10" s="9"/>
       <c r="O10" s="9"/>
     </row>
     <row r="11" ht="100" customHeight="1">
-      <c r="A11" s="26"/>
-      <c r="B11" s="36"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="29"/>
-      <c r="K11" s="29"/>
-      <c r="L11" s="29"/>
+      <c r="A11" s="30"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="33"/>
+      <c r="L11" s="33"/>
       <c r="M11" s="9"/>
       <c r="N11" s="9"/>
       <c r="O11" s="9"/>
     </row>
     <row r="12" ht="100" customHeight="1">
-      <c r="A12" s="26"/>
-      <c r="B12" s="36"/>
-      <c r="C12" s="28"/>
+      <c r="A12" s="30"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="32"/>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
@@ -2886,25 +2933,25 @@
       <c r="O12" s="9"/>
     </row>
     <row r="13" ht="100" customHeight="1">
-      <c r="A13" s="26"/>
-      <c r="B13" s="36"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
+      <c r="A13" s="30"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
-      <c r="G13" s="28"/>
+      <c r="G13" s="32"/>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
-      <c r="J13" s="28"/>
+      <c r="J13" s="32"/>
       <c r="K13" s="9"/>
       <c r="L13" s="9"/>
-      <c r="M13" s="28"/>
+      <c r="M13" s="32"/>
       <c r="N13" s="9"/>
       <c r="O13" s="9"/>
     </row>
     <row r="14" ht="100" customHeight="1">
       <c r="A14" s="7"/>
-      <c r="B14" s="37"/>
+      <c r="B14" s="41"/>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
@@ -3041,165 +3088,165 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="29.5" style="38" customWidth="1"/>
-    <col min="2" max="15" width="16.3516" style="38" customWidth="1"/>
-    <col min="16" max="16384" width="16.3516" style="38" customWidth="1"/>
+    <col min="1" max="1" width="29.5" style="42" customWidth="1"/>
+    <col min="2" max="15" width="16.3516" style="42" customWidth="1"/>
+    <col min="16" max="16384" width="16.3516" style="42" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="100" customHeight="1">
-      <c r="A1" t="s" s="20">
-        <v>77</v>
-      </c>
-      <c r="B1" t="s" s="21">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s" s="21">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s" s="21">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s" s="21">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s" s="21">
-        <v>9</v>
-      </c>
-      <c r="G1" t="s" s="21">
-        <v>10</v>
-      </c>
-      <c r="H1" t="s" s="21">
-        <v>11</v>
-      </c>
-      <c r="I1" t="s" s="21">
-        <v>12</v>
-      </c>
-      <c r="J1" t="s" s="21">
-        <v>13</v>
-      </c>
-      <c r="K1" t="s" s="21">
+      <c r="A1" t="s" s="24">
+        <v>86</v>
+      </c>
+      <c r="B1" t="s" s="25">
         <v>14</v>
       </c>
-      <c r="L1" t="s" s="21">
+      <c r="C1" t="s" s="25">
         <v>15</v>
       </c>
-      <c r="M1" t="s" s="21">
+      <c r="D1" t="s" s="25">
         <v>16</v>
       </c>
-      <c r="N1" t="s" s="21">
+      <c r="E1" t="s" s="25">
         <v>17</v>
       </c>
-      <c r="O1" t="s" s="21">
+      <c r="F1" t="s" s="25">
         <v>18</v>
       </c>
+      <c r="G1" t="s" s="25">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s" s="25">
+        <v>20</v>
+      </c>
+      <c r="I1" t="s" s="25">
+        <v>21</v>
+      </c>
+      <c r="J1" t="s" s="25">
+        <v>22</v>
+      </c>
+      <c r="K1" t="s" s="25">
+        <v>23</v>
+      </c>
+      <c r="L1" t="s" s="25">
+        <v>24</v>
+      </c>
+      <c r="M1" t="s" s="25">
+        <v>25</v>
+      </c>
+      <c r="N1" t="s" s="25">
+        <v>26</v>
+      </c>
+      <c r="O1" t="s" s="25">
+        <v>27</v>
+      </c>
     </row>
     <row r="2" ht="100" customHeight="1">
-      <c r="A2" t="s" s="22">
-        <v>78</v>
-      </c>
-      <c r="B2" t="s" s="39">
-        <v>79</v>
-      </c>
-      <c r="C2" t="s" s="40">
-        <v>80</v>
-      </c>
-      <c r="D2" t="s" s="40">
-        <v>81</v>
-      </c>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" t="s" s="40">
-        <v>82</v>
-      </c>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" t="s" s="40">
-        <v>83</v>
-      </c>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" t="s" s="40">
-        <v>84</v>
-      </c>
-      <c r="N2" s="42"/>
-      <c r="O2" s="42"/>
+      <c r="A2" t="s" s="26">
+        <v>87</v>
+      </c>
+      <c r="B2" t="s" s="43">
+        <v>88</v>
+      </c>
+      <c r="C2" t="s" s="44">
+        <v>89</v>
+      </c>
+      <c r="D2" t="s" s="44">
+        <v>90</v>
+      </c>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" t="s" s="44">
+        <v>91</v>
+      </c>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" t="s" s="44">
+        <v>92</v>
+      </c>
+      <c r="K2" s="45"/>
+      <c r="L2" s="45"/>
+      <c r="M2" t="s" s="44">
+        <v>93</v>
+      </c>
+      <c r="N2" s="46"/>
+      <c r="O2" s="46"/>
     </row>
     <row r="3" ht="100" customHeight="1">
-      <c r="A3" t="s" s="26">
-        <v>85</v>
-      </c>
-      <c r="B3" t="s" s="36">
-        <v>86</v>
-      </c>
-      <c r="C3" t="s" s="43">
-        <v>87</v>
-      </c>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="45"/>
-      <c r="N3" s="45"/>
-      <c r="O3" s="45"/>
+      <c r="A3" t="s" s="30">
+        <v>94</v>
+      </c>
+      <c r="B3" t="s" s="40">
+        <v>95</v>
+      </c>
+      <c r="C3" t="s" s="47">
+        <v>96</v>
+      </c>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="49"/>
     </row>
     <row r="4" ht="100" customHeight="1">
-      <c r="A4" t="s" s="26">
-        <v>88</v>
-      </c>
-      <c r="B4" t="s" s="36">
-        <v>89</v>
-      </c>
-      <c r="C4" t="s" s="43">
-        <v>90</v>
-      </c>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
-      <c r="K4" s="45"/>
-      <c r="L4" s="45"/>
-      <c r="M4" s="45"/>
-      <c r="N4" s="45"/>
-      <c r="O4" s="45"/>
+      <c r="A4" t="s" s="30">
+        <v>97</v>
+      </c>
+      <c r="B4" t="s" s="40">
+        <v>98</v>
+      </c>
+      <c r="C4" t="s" s="47">
+        <v>99</v>
+      </c>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="49"/>
+      <c r="M4" s="49"/>
+      <c r="N4" s="49"/>
+      <c r="O4" s="49"/>
     </row>
     <row r="5" ht="100" customHeight="1">
-      <c r="A5" t="s" s="26">
-        <v>91</v>
-      </c>
-      <c r="B5" t="s" s="36">
-        <v>92</v>
-      </c>
-      <c r="C5" t="s" s="43">
-        <v>93</v>
-      </c>
-      <c r="D5" t="s" s="43">
-        <v>94</v>
-      </c>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" t="s" s="43">
-        <v>95</v>
-      </c>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
-      <c r="J5" t="s" s="43">
-        <v>96</v>
-      </c>
-      <c r="K5" s="45"/>
-      <c r="L5" s="45"/>
-      <c r="M5" t="s" s="43">
-        <v>97</v>
-      </c>
-      <c r="N5" s="45"/>
-      <c r="O5" s="45"/>
+      <c r="A5" t="s" s="30">
+        <v>100</v>
+      </c>
+      <c r="B5" t="s" s="40">
+        <v>101</v>
+      </c>
+      <c r="C5" t="s" s="47">
+        <v>102</v>
+      </c>
+      <c r="D5" t="s" s="47">
+        <v>103</v>
+      </c>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" t="s" s="47">
+        <v>104</v>
+      </c>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
+      <c r="J5" t="s" s="47">
+        <v>105</v>
+      </c>
+      <c r="K5" s="49"/>
+      <c r="L5" s="49"/>
+      <c r="M5" t="s" s="47">
+        <v>106</v>
+      </c>
+      <c r="N5" s="49"/>
+      <c r="O5" s="49"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>